<commit_message>
add auto spliting dataset
</commit_message>
<xml_diff>
--- a/parameter.xlsx
+++ b/parameter.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohanesisa/skripsi/sentiment-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B90790-3DEA-D546-AB7D-50CF880A0A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0056702F-8C4E-EC43-B291-DC10EEC8E380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="-18720" windowWidth="28040" windowHeight="16580" xr2:uid="{65584DBE-D15F-2745-A562-9FEA8BD94068}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{65584DBE-D15F-2745-A562-9FEA8BD94068}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -433,47 +433,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144E887B-1E82-1447-87E3-9E900A1BF629}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="144" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1">
+        <v>-15</v>
+      </c>
+      <c r="B1">
+        <v>-14</v>
+      </c>
+      <c r="C1">
+        <v>-13</v>
+      </c>
+      <c r="D1">
+        <v>-12</v>
+      </c>
+      <c r="E1">
+        <v>-11</v>
+      </c>
+      <c r="F1">
+        <v>-10</v>
+      </c>
+      <c r="G1">
+        <v>-9</v>
+      </c>
+      <c r="H1">
+        <v>-8</v>
+      </c>
+      <c r="I1">
         <v>-7</v>
       </c>
-      <c r="B1">
+      <c r="J1">
         <v>-6</v>
       </c>
-      <c r="C1">
+      <c r="K1">
         <v>-5</v>
       </c>
-      <c r="D1">
+      <c r="L1">
         <v>-4</v>
       </c>
-      <c r="E1">
+      <c r="M1">
         <v>-3</v>
       </c>
-      <c r="F1">
+      <c r="N1">
         <v>-2</v>
       </c>
-      <c r="G1">
+      <c r="O1">
         <v>-1</v>
       </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>1</v>
-      </c>
-      <c r="J1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>1</v>
+      </c>
+      <c r="R1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -504,82 +528,162 @@
       <c r="J2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>POWER(A2,A1)</f>
-        <v>9.9999999999999995E-8</v>
+        <f t="shared" ref="A3:H3" si="0">POWER(A2,A1)</f>
+        <v>1.0000000000000001E-15</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:J3" si="0">POWER(B2,B1)</f>
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>1E-14</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>1E-13</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1E-4</v>
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>1E-3</v>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>1E-10</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1E-8</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>POWER(I2,I1)</f>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J3:R3" si="1">POWER(J2,J1)</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>-15</v>
+      </c>
+      <c r="B5">
+        <v>-14</v>
+      </c>
+      <c r="C5">
+        <v>-13</v>
+      </c>
+      <c r="D5">
+        <v>-12</v>
+      </c>
+      <c r="E5">
+        <v>-11</v>
+      </c>
+      <c r="F5">
+        <v>-10</v>
+      </c>
+      <c r="G5">
+        <v>-9</v>
+      </c>
+      <c r="H5">
+        <v>-8</v>
+      </c>
+      <c r="I5">
         <v>-7</v>
       </c>
-      <c r="B5">
+      <c r="J5">
         <v>-6</v>
       </c>
-      <c r="C5">
+      <c r="K5">
         <v>-5</v>
       </c>
-      <c r="D5">
+      <c r="L5">
         <v>-4</v>
       </c>
-      <c r="E5">
+      <c r="M5">
         <v>-3</v>
       </c>
-      <c r="F5">
+      <c r="N5">
         <v>-2</v>
       </c>
-      <c r="G5">
+      <c r="O5">
         <v>-1</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -610,50 +714,106 @@
       <c r="J6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f>POWER(A6,A5)</f>
+        <f t="shared" ref="A7:H7" si="2">POWER(A6,A5)</f>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="2"/>
+        <v>6.103515625E-5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>1.220703125E-4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>4.8828125E-4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="I7">
+        <f>POWER(I6,I5)</f>
         <v>7.8125E-3</v>
       </c>
-      <c r="B7">
-        <f t="shared" ref="B7" si="1">POWER(B6,B5)</f>
+      <c r="J7">
+        <f t="shared" ref="J7" si="3">POWER(J6,J5)</f>
         <v>1.5625E-2</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7" si="2">POWER(C6,C5)</f>
+      <c r="K7">
+        <f t="shared" ref="K7" si="4">POWER(K6,K5)</f>
         <v>3.125E-2</v>
       </c>
-      <c r="D7">
-        <f t="shared" ref="D7" si="3">POWER(D6,D5)</f>
+      <c r="L7">
+        <f t="shared" ref="L7" si="5">POWER(L6,L5)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E7">
-        <f t="shared" ref="E7" si="4">POWER(E6,E5)</f>
+      <c r="M7">
+        <f t="shared" ref="M7" si="6">POWER(M6,M5)</f>
         <v>0.125</v>
       </c>
-      <c r="F7">
-        <f t="shared" ref="F7" si="5">POWER(F6,F5)</f>
+      <c r="N7">
+        <f t="shared" ref="N7" si="7">POWER(N6,N5)</f>
         <v>0.25</v>
       </c>
-      <c r="G7">
-        <f t="shared" ref="G7" si="6">POWER(G6,G5)</f>
+      <c r="O7">
+        <f t="shared" ref="O7" si="8">POWER(O6,O5)</f>
         <v>0.5</v>
       </c>
-      <c r="H7">
-        <f t="shared" ref="H7" si="7">POWER(H6,H5)</f>
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ref="I7" si="8">POWER(I6,I5)</f>
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <f t="shared" ref="J7" si="9">POWER(J6,J5)</f>
+      <c r="P7">
+        <f t="shared" ref="P7" si="9">POWER(P6,P5)</f>
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7" si="10">POWER(Q6,Q5)</f>
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7" si="11">POWER(R6,R5)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -679,7 +839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -700,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -722,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -733,21 +893,21 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
       <c r="H14">
         <f>B14*C14*D14*G14</f>
-        <v>1500</v>
+        <v>2700</v>
       </c>
       <c r="I14">
         <f>D14</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -758,24 +918,24 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G15">
         <v>3</v>
       </c>
       <c r="H15">
         <f>B15*C15*E15*F15*G15</f>
-        <v>15000</v>
+        <v>48600</v>
       </c>
       <c r="I15">
         <f>E15*F15</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -803,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>(COUNT($B$17:$B$24)*(A17))+(B17+1)</f>
+        <f t="shared" ref="C17:C42" si="12">(COUNT($B$17:$B$24)*(A17))+(B17+1)</f>
         <v>1</v>
       </c>
       <c r="E17">
@@ -827,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <f>(COUNT($B$17:$B$24)*(A18))+(B18+1)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="E18">
@@ -858,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <f>(COUNT($B$17:$B$24)*(A19))+(B19+1)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="E19">
@@ -874,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:I77" si="10">($F$17*E19)+($G$17*F19)+($H$17*G19)+(H19+1)</f>
+        <f t="shared" ref="I19:I77" si="13">($F$17*E19)+($G$17*F19)+($H$17*G19)+(H19+1)</f>
         <v>2</v>
       </c>
       <c r="J19">
@@ -889,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <f>(COUNT($B$17:$B$24)*(A20))+(B20+1)</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="E20">
@@ -905,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="I20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="J20">
@@ -920,7 +1080,7 @@
         <v>4</v>
       </c>
       <c r="C21">
-        <f>(COUNT($B$17:$B$24)*(A21))+(B21+1)</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="E21">
@@ -936,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="J21">
@@ -951,7 +1111,7 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <f>(COUNT($B$17:$B$24)*(A22))+(B22+1)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="E22">
@@ -967,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="J22">
@@ -982,7 +1142,7 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <f>(COUNT($B$17:$B$24)*(A23))+(B23+1)</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="E23">
@@ -998,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="I23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="J23">
@@ -1013,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="C24">
-        <f>(COUNT($B$17:$B$24)*(A24))+(B24+1)</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="E24">
@@ -1029,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="J24">
@@ -1044,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>(COUNT($B$17:$B$24)*(A25))+(B25+1)</f>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="E25">
@@ -1060,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="J25">
@@ -1075,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <f>(COUNT($B$17:$B$24)*(A26))+(B26+1)</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="E26">
@@ -1091,7 +1251,7 @@
         <v>2</v>
       </c>
       <c r="I26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="J26">
@@ -1106,7 +1266,7 @@
         <v>2</v>
       </c>
       <c r="C27">
-        <f>(COUNT($B$17:$B$24)*(A27))+(B27+1)</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="E27">
@@ -1122,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="J27">
@@ -1137,7 +1297,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <f>(COUNT($B$17:$B$24)*(A28))+(B28+1)</f>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="E28">
@@ -1153,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="J28">
@@ -1168,7 +1328,7 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <f>(COUNT($B$17:$B$24)*(A29))+(B29+1)</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="E29">
@@ -1184,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="J29">
@@ -1199,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <f>(COUNT($B$17:$B$24)*(A30))+(B30+1)</f>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="E30">
@@ -1215,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="J30">
@@ -1230,7 +1390,7 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <f>(COUNT($B$17:$B$24)*(A31))+(B31+1)</f>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
       <c r="E31">
@@ -1246,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="J31">
@@ -1261,7 +1421,7 @@
         <v>7</v>
       </c>
       <c r="C32">
-        <f>(COUNT($B$17:$B$24)*(A32))+(B32+1)</f>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
       <c r="E32">
@@ -1277,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="I32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="J32">
@@ -1292,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>(COUNT($B$17:$B$24)*(A33))+(B33+1)</f>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
       <c r="E33">
@@ -1308,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="J33">
@@ -1323,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <f>(COUNT($B$17:$B$24)*(A34))+(B34+1)</f>
+        <f t="shared" si="12"/>
         <v>18</v>
       </c>
       <c r="E34">
@@ -1339,7 +1499,7 @@
         <v>1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="J34">
@@ -1354,7 +1514,7 @@
         <v>2</v>
       </c>
       <c r="C35">
-        <f>(COUNT($B$17:$B$24)*(A35))+(B35+1)</f>
+        <f t="shared" si="12"/>
         <v>19</v>
       </c>
       <c r="E35">
@@ -1370,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="I35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="J35">
@@ -1385,7 +1545,7 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <f>(COUNT($B$17:$B$24)*(A36))+(B36+1)</f>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="E36">
@@ -1401,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="J36">
@@ -1416,7 +1576,7 @@
         <v>4</v>
       </c>
       <c r="C37">
-        <f>(COUNT($B$17:$B$24)*(A37))+(B37+1)</f>
+        <f t="shared" si="12"/>
         <v>21</v>
       </c>
       <c r="E37">
@@ -1432,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="I37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="J37">
@@ -1447,7 +1607,7 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <f>(COUNT($B$17:$B$24)*(A38))+(B38+1)</f>
+        <f t="shared" si="12"/>
         <v>22</v>
       </c>
       <c r="E38">
@@ -1463,7 +1623,7 @@
         <v>2</v>
       </c>
       <c r="I38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
       <c r="J38">
@@ -1478,7 +1638,7 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <f>(COUNT($B$17:$B$24)*(A39))+(B39+1)</f>
+        <f t="shared" si="12"/>
         <v>23</v>
       </c>
       <c r="E39">
@@ -1494,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="J39">
@@ -1509,7 +1669,7 @@
         <v>7</v>
       </c>
       <c r="C40">
-        <f>(COUNT($B$17:$B$24)*(A40))+(B40+1)</f>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
       <c r="E40">
@@ -1525,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="I40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="J40">
@@ -1540,7 +1700,7 @@
         <v>8</v>
       </c>
       <c r="C41">
-        <f>(COUNT($B$17:$B$24)*(A41))+(B41+1)</f>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
       <c r="E41">
@@ -1556,7 +1716,7 @@
         <v>2</v>
       </c>
       <c r="I41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="J41">
@@ -1571,7 +1731,7 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <f>(COUNT($B$17:$B$24)*(A42))+(B42+1)</f>
+        <f t="shared" si="12"/>
         <v>26</v>
       </c>
       <c r="E42">
@@ -1587,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="J42">
@@ -1608,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="J43">
@@ -1629,7 +1789,7 @@
         <v>2</v>
       </c>
       <c r="I44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="J44">
@@ -1650,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="J45">
@@ -1671,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="J46">
@@ -1692,7 +1852,7 @@
         <v>2</v>
       </c>
       <c r="I47">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="J47">
@@ -1713,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="J48">
@@ -1734,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="I49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="J49">
@@ -1755,7 +1915,7 @@
         <v>2</v>
       </c>
       <c r="I50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="J50">
@@ -1776,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="J51">
@@ -1797,7 +1957,7 @@
         <v>1</v>
       </c>
       <c r="I52">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="J52">
@@ -1818,7 +1978,7 @@
         <v>2</v>
       </c>
       <c r="I53">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="J53">
@@ -1839,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="J54">
@@ -1860,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="I55">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="J55">
@@ -1881,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="I56">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="J56">
@@ -1902,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="J57">
@@ -1923,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="I58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
       <c r="J58">
@@ -1944,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="I59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="J59">
@@ -1965,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="J60">
@@ -1986,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="I61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="J61">
@@ -2007,7 +2167,7 @@
         <v>2</v>
       </c>
       <c r="I62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="J62">
@@ -2028,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="J63">
@@ -2049,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="I64">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="J64">
@@ -2070,7 +2230,7 @@
         <v>2</v>
       </c>
       <c r="I65">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="J65">
@@ -2091,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="J66">
@@ -2112,7 +2272,7 @@
         <v>1</v>
       </c>
       <c r="I67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="J67">
@@ -2133,7 +2293,7 @@
         <v>2</v>
       </c>
       <c r="I68">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>31</v>
       </c>
       <c r="J68">
@@ -2154,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>32</v>
       </c>
       <c r="J69">
@@ -2175,7 +2335,7 @@
         <v>1</v>
       </c>
       <c r="I70">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>33</v>
       </c>
       <c r="J70">
@@ -2196,7 +2356,7 @@
         <v>2</v>
       </c>
       <c r="I71">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="J71">
@@ -2217,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>35</v>
       </c>
       <c r="J72">
@@ -2238,7 +2398,7 @@
         <v>1</v>
       </c>
       <c r="I73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="J73">
@@ -2259,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="I74">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="J74">
@@ -2280,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="I75">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>38</v>
       </c>
       <c r="J75">
@@ -2301,7 +2461,7 @@
         <v>1</v>
       </c>
       <c r="I76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>39</v>
       </c>
       <c r="J76">
@@ -2322,7 +2482,7 @@
         <v>2</v>
       </c>
       <c r="I77">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>40</v>
       </c>
       <c r="J77">

</xml_diff>